<commit_message>
added forecasted filepath for prevalence
</commit_message>
<xml_diff>
--- a/docs/source/gbd2017_models/causes/neoplasms/breast_cancer_with_stage0/filepaths_c429_forecast.xlsx
+++ b/docs/source/gbd2017_models/causes/neoplasms/breast_cancer_with_stage0/filepaths_c429_forecast.xlsx
@@ -53,9 +53,6 @@
     <t>/ihme/costeffectiveness/vivarium_csu_cancer/429_ets_mortality.nc</t>
   </si>
   <si>
-    <t>to be determined</t>
-  </si>
-  <si>
     <t>acmr</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>percent</t>
+  </si>
+  <si>
+    <t>/ihme/costeffectiveness/vivarium_csu_cancer/429_ets_prevalence_beta_8_phi_89.nc</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +413,7 @@
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -424,10 +424,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -441,13 +441,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -455,10 +455,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -469,10 +469,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -480,16 +480,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected forecast data unit description
</commit_message>
<xml_diff>
--- a/docs/source/gbd2017_models/causes/neoplasms/breast_cancer_with_stage0/filepaths_c429_forecast.xlsx
+++ b/docs/source/gbd2017_models/causes/neoplasms/breast_cancer_with_stage0/filepaths_c429_forecast.xlsx
@@ -5,20 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicoly\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\vivarium_research\docs\source\gbd2017_models\causes\neoplasms\breast_cancer_with_stage0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="2370" windowHeight="0" tabRatio="849" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="2370" windowHeight="0" tabRatio="931" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="filepaths" sheetId="1" r:id="rId1"/>
-    <sheet name="acmr_294" sheetId="3" r:id="rId2"/>
-    <sheet name="csmr_c429" sheetId="6" r:id="rId3"/>
-    <sheet name="incidence_c429" sheetId="7" r:id="rId4"/>
-    <sheet name="prevalence_c429" sheetId="2" r:id="rId5"/>
-    <sheet name="age_groups" sheetId="4" r:id="rId6"/>
-    <sheet name="location_id" sheetId="5" r:id="rId7"/>
+    <sheet name="csmr_c429" sheetId="6" r:id="rId2"/>
+    <sheet name="incidence_c429" sheetId="7" r:id="rId3"/>
+    <sheet name="prevalence_c429" sheetId="2" r:id="rId4"/>
+    <sheet name="age_groups" sheetId="4" r:id="rId5"/>
+    <sheet name="location_id" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="102">
   <si>
     <t>forcasted 2020-2040</t>
   </si>
@@ -326,16 +325,16 @@
     <t>acmr 294</t>
   </si>
   <si>
-    <t>after exp transformation: percentage stratified by age, sex, location year</t>
-  </si>
-  <si>
-    <t>This is the log(acmr). After exp transformation: all-cause mortality rate as death per person-years stratified by age, sex, location year</t>
-  </si>
-  <si>
-    <t>This is the log(csmr). After exp transformation: cause specific mortality rate as death per person year stratified by age, sex, location year</t>
-  </si>
-  <si>
-    <t>This is the log(incidence rate). After exp transformation: incidence rate per person year stratified by age, sex, location year</t>
+    <t>float, rate space</t>
+  </si>
+  <si>
+    <t>cause specific mortality rate as death per person year stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> incidence rate per person year stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>after exp transformation: proportion stratified by age, sex, location year</t>
   </si>
 </sst>
 </file>
@@ -431,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -447,9 +446,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -865,166 +861,162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>17</v>
       </c>
-      <c r="F3" s="12">
-        <v>23</v>
-      </c>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="11">
+        <v>17</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>2</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>33</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>33</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>51</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>51</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>1000</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>1000</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <f>PRODUCT(E3:E7)</f>
         <v>57222000</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1032,169 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="12">
-        <v>17</v>
-      </c>
-      <c r="F3" s="12">
-        <v>17</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="13">
-        <v>2</v>
-      </c>
-      <c r="F4" s="13">
-        <v>2</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="12">
-        <v>33</v>
-      </c>
-      <c r="F5" s="12">
-        <v>33</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="12">
-        <v>51</v>
-      </c>
-      <c r="F6" s="12">
-        <v>51</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1000</v>
-      </c>
-      <c r="F7" s="13">
-        <v>1000</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="18">
-        <f>PRODUCT(E3:E7)</f>
-        <v>57222000</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="17"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G8"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H13:H15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,153 +1040,153 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>17</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>17</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>2</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>33</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>33</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>51</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>51</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>1000</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>1000</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="18">
+      <c r="C8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="17">
         <f>PRODUCT(E3:E7)</f>
         <v>57222000</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,141 +1201,141 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>17</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>17</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>2</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>33</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>33</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>51</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>51</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>1000</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>1000</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="18">
+      <c r="D8" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="17">
         <f>PRODUCT(E3:E7)</f>
         <v>57222000</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1512,12 +1343,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,7 +1637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I35"/>
   <sheetViews>
@@ -1825,21 +1656,21 @@
       <c r="B2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>354</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>361</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>61</v>
       </c>
       <c r="D4" s="2"/>
@@ -1850,250 +1681,250 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>491</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>492</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>493</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>494</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>495</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="19">
+      <c r="B10" s="18">
         <v>496</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>497</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>498</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>499</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>500</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="19">
+      <c r="B15" s="18">
         <v>501</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>502</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>503</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>504</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>505</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="19">
+      <c r="B20" s="18">
         <v>506</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>507</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>508</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <v>509</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>510</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>511</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <v>512</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="10">
+      <c r="B27" s="9">
         <v>513</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <v>514</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="9">
+      <c r="B29" s="8">
         <v>515</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>516</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="19">
+      <c r="B31" s="18">
         <v>517</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="19" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="9">
+      <c r="B32" s="8">
         <v>518</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="10">
+      <c r="B33" s="9">
         <v>519</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="16" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="10">
+      <c r="B34" s="9">
         <v>520</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="9">
+      <c r="B35" s="8">
         <v>521</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="16" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
formated rst file to show screening scale up
</commit_message>
<xml_diff>
--- a/docs/source/gbd2017_models/causes/neoplasms/breast_cancer_with_stage0/filepaths_c429_forecast.xlsx
+++ b/docs/source/gbd2017_models/causes/neoplasms/breast_cancer_with_stage0/filepaths_c429_forecast.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="2370" windowHeight="0" tabRatio="931" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="2370" windowHeight="0" tabRatio="931"/>
   </bookViews>
   <sheets>
     <sheet name="filepaths" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>/ihme/costeffectiveness/vivarium_csu_cancer/429_ets_mortality.nc</t>
   </si>
   <si>
-    <t>to be determined</t>
-  </si>
-  <si>
     <t>/ihme/costeffectiveness/vivarium_csu_cancer/294_ets_mortality_beta_8_phi_89.nc</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>draw-level</t>
   </si>
   <si>
-    <t>percent</t>
-  </si>
-  <si>
     <t>age_group</t>
   </si>
   <si>
@@ -335,6 +329,12 @@
   </si>
   <si>
     <t>after exp transformation: proportion stratified by age, sex, location year</t>
+  </si>
+  <si>
+    <t>log(prevalence), proportion</t>
+  </si>
+  <si>
+    <t>/ihme/costeffectiveness/vivarium_csu_cancer/429_ets_prevalence_beta_8_phi_89.nc</t>
   </si>
 </sst>
 </file>
@@ -764,15 +764,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -785,10 +785,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -802,24 +802,24 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -830,10 +830,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -841,16 +841,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +864,7 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,33 +880,33 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="11">
         <v>17</v>
@@ -915,18 +915,18 @@
         <v>17</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="12">
         <v>2</v>
@@ -935,18 +935,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" s="11">
         <v>33</v>
@@ -955,18 +955,18 @@
         <v>33</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="11">
         <v>51</v>
@@ -975,18 +975,18 @@
         <v>51</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="E7" s="12">
         <v>1000</v>
@@ -995,18 +995,18 @@
         <v>1000</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E8" s="17">
         <f>PRODUCT(E3:E7)</f>
@@ -1025,14 +1025,14 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -1041,33 +1041,33 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="11">
         <v>17</v>
@@ -1076,18 +1076,18 @@
         <v>17</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="12">
         <v>2</v>
@@ -1096,18 +1096,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" s="11">
         <v>33</v>
@@ -1116,18 +1116,18 @@
         <v>33</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="11">
         <v>51</v>
@@ -1136,18 +1136,18 @@
         <v>51</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="E7" s="12">
         <v>1000</v>
@@ -1156,18 +1156,18 @@
         <v>1000</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="E8" s="17">
         <f>PRODUCT(E3:E7)</f>
@@ -1185,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,33 +1202,33 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="11">
         <v>17</v>
@@ -1237,18 +1237,18 @@
         <v>17</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="12">
         <v>2</v>
@@ -1257,18 +1257,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" s="11">
         <v>33</v>
@@ -1277,18 +1277,18 @@
         <v>33</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="11">
         <v>51</v>
@@ -1297,18 +1297,18 @@
         <v>51</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="E7" s="12">
         <v>1000</v>
@@ -1317,18 +1317,18 @@
         <v>1000</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="D8" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8" s="17">
         <f>PRODUCT(E3:E7)</f>
@@ -1361,16 +1361,16 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -1380,7 +1380,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="6">
         <v>15</v>
@@ -1396,7 +1396,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7">
         <v>20</v>
@@ -1412,7 +1412,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6">
         <v>25</v>
@@ -1427,7 +1427,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>30</v>
@@ -1442,7 +1442,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="6">
         <v>35</v>
@@ -1457,7 +1457,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="7">
         <v>40</v>
@@ -1472,7 +1472,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6">
         <v>45</v>
@@ -1487,7 +1487,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="7">
         <v>50</v>
@@ -1502,7 +1502,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="6">
         <v>55</v>
@@ -1517,7 +1517,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="7">
         <v>60</v>
@@ -1532,7 +1532,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="6">
         <v>65</v>
@@ -1547,7 +1547,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" s="7">
         <v>70</v>
@@ -1562,7 +1562,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="6">
         <v>75</v>
@@ -1577,7 +1577,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="7">
         <v>80</v>
@@ -1592,7 +1592,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="6">
         <v>85</v>
@@ -1607,7 +1607,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="7">
         <v>90</v>
@@ -1622,7 +1622,7 @@
         <v>235</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="7">
         <v>95</v>
@@ -1641,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,7 +1654,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="16"/>
     </row>
@@ -1663,7 +1663,7 @@
         <v>354</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
         <v>361</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1685,7 +1685,7 @@
         <v>491</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
         <v>492</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -1701,7 +1701,7 @@
         <v>493</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>494</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -1717,7 +1717,7 @@
         <v>495</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -1725,7 +1725,7 @@
         <v>496</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -1733,7 +1733,7 @@
         <v>497</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -1741,7 +1741,7 @@
         <v>498</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>499</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
         <v>500</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>501</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -1773,7 +1773,7 @@
         <v>502</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -1781,7 +1781,7 @@
         <v>503</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -1789,7 +1789,7 @@
         <v>504</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -1797,7 +1797,7 @@
         <v>505</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
         <v>506</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -1813,7 +1813,7 @@
         <v>507</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
         <v>508</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -1829,7 +1829,7 @@
         <v>509</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
         <v>510</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>511</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -1853,7 +1853,7 @@
         <v>512</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>513</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -1869,7 +1869,7 @@
         <v>514</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>515</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -1885,7 +1885,7 @@
         <v>516</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -1893,7 +1893,7 @@
         <v>517</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -1901,7 +1901,7 @@
         <v>518</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -1909,7 +1909,7 @@
         <v>519</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -1917,7 +1917,7 @@
         <v>520</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -1925,7 +1925,7 @@
         <v>521</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>